<commit_message>
Included data driven behavior. Now reading the data from excel
</commit_message>
<xml_diff>
--- a/e2e/protractor/testdata/TestData.xlsx
+++ b/e2e/protractor/testdata/TestData.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="RegistrationPage" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>username</t>
   </si>
@@ -27,12 +27,6 @@
     <t>password</t>
   </si>
   <si>
-    <t>Runmode</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>first name</t>
   </si>
   <si>
@@ -54,12 +48,6 @@
     <t>Expected Result</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Mohan</t>
-  </si>
-  <si>
     <t>T</t>
   </si>
   <si>
@@ -67,6 +55,15 @@
   </si>
   <si>
     <t>^^$ABC</t>
+  </si>
+  <si>
+    <t>Testcase description</t>
+  </si>
+  <si>
+    <t>Valid values verification</t>
+  </si>
+  <si>
+    <t>mohan</t>
   </si>
 </sst>
 </file>
@@ -387,11 +384,12 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="38" customWidth="1"/>
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.28515625" customWidth="1"/>
     <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
@@ -399,13 +397,13 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -414,49 +412,44 @@
         <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
         <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576">
-      <formula1>"Yes, No"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>